<commit_message>
fix to export surveys
</commit_message>
<xml_diff>
--- a/files/encuestas.xlsx
+++ b/files/encuestas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,12 +461,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>NOMBRE</t>
+          <t>contact_name</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>CELULAR</t>
+          <t>contact_phone</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -499,19 +499,47 @@
           <t>update test</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Encuesta 1</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2225547275</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
           <t>CANCELED</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>35</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>693bbd42-82e6-4da8-a809-804be6d24f52</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-12-10T12:59:04.124702-06:00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>COMPLAINT</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>contact_name 1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>contact_phone 1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>IN_PROGRESS</t>
         </is>
       </c>
     </row>

</xml_diff>